<commit_message>
Adicionando material para consumo e provimento de operações IIB
</commit_message>
<xml_diff>
--- a/Pessoal/atalada/atalada.xlsx
+++ b/Pessoal/atalada/atalada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://banco365-my.sharepoint.com/personal/murilo_asantos_bb_com_br/Documents/Área de Trabalho/repo-murilo-bb/repo-murilo-bb/Pessoal/atalada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_F25DC773A252ABDACC1048DDB19E6B945BDE58FA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4DF8B6F-CDB1-4E5E-8508-B9018E088C47}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_F25DC773A252ABDACC1048DDB19E6B945BDE58FA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A47BCBB3-C39B-4A31-BE35-795D28944B9C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Impessoal</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>Nary0000</t>
+  </si>
+  <si>
+    <t>fgi-h</t>
+  </si>
+  <si>
+    <t>nary1408</t>
+  </si>
+  <si>
+    <t>fgi-p</t>
+  </si>
+  <si>
+    <t>murilo121212</t>
   </si>
 </sst>
 </file>
@@ -98,6 +110,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -363,15 +379,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -379,7 +400,7 @@
         <v>42349860</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -387,7 +408,7 @@
         <v>42349866</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -395,7 +416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -403,12 +424,34 @@
         <v>42349866</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionado estudos com map e json
</commit_message>
<xml_diff>
--- a/Pessoal/atalada/atalada.xlsx
+++ b/Pessoal/atalada/atalada.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://banco365-my.sharepoint.com/personal/murilo_asantos_bb_com_br/Documents/Área de Trabalho/repo-murilo-bb/repo-murilo-bb/Pessoal/atalada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="11_F25DC773A252ABDACC1048DDB19E6B945BDE58FA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA4B6413-24B2-4AEA-9352-337EE542444B}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_F25DC773A252ABDACC1048DDB19E6B945BDE58FA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B09810F7-F1AA-49C8-8B2D-1A6CFD0CB01D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>